<commit_message>
Add icon and finalize yamls and build
</commit_message>
<xml_diff>
--- a/.private/docs/Approved Title/Appendices/Lakbay - Appendices.xlsx
+++ b/.private/docs/Approved Title/Appendices/Lakbay - Appendices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NILA\Documents\BSIT-Capstone\.private\docs\Approved Title\Appendices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD866790-AC82-4B6E-AD59-5F20F62B8205}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73F4968-4199-40C4-A64E-F5CA417C4830}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" firstSheet="3" activeTab="6" xr2:uid="{A35BE531-B805-4D43-AE67-6216240D3748}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" firstSheet="3" activeTab="4" xr2:uid="{A35BE531-B805-4D43-AE67-6216240D3748}"/>
   </bookViews>
   <sheets>
     <sheet name="Flowchart of Information Module" sheetId="1" r:id="rId1"/>
@@ -8683,8 +8683,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3829082" y="3680260"/>
-          <a:ext cx="166450" cy="91440"/>
+          <a:off x="3900613" y="3909555"/>
+          <a:ext cx="169560" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8698,7 +8698,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="166450" y="45720"/>
+                <a:pt x="169560" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -8739,8 +8739,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2830377" y="3680260"/>
-          <a:ext cx="166450" cy="91440"/>
+          <a:off x="2883250" y="3909555"/>
+          <a:ext cx="169560" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8754,7 +8754,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="166450" y="45720"/>
+                <a:pt x="169560" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -8795,8 +8795,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1831671" y="3547045"/>
-          <a:ext cx="166450" cy="178934"/>
+          <a:off x="1865888" y="3772998"/>
+          <a:ext cx="169560" cy="182277"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8810,13 +8810,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="83225" y="0"/>
+                <a:pt x="84780" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="83225" y="178934"/>
+                <a:pt x="84780" y="182277"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="166450" y="178934"/>
+                <a:pt x="169560" y="182277"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -8857,8 +8857,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3829082" y="3322391"/>
-          <a:ext cx="166450" cy="91440"/>
+          <a:off x="3900613" y="3545000"/>
+          <a:ext cx="169560" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8872,7 +8872,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="166450" y="45720"/>
+                <a:pt x="169560" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -8913,8 +8913,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2830377" y="3322391"/>
-          <a:ext cx="166450" cy="91440"/>
+          <a:off x="2883250" y="3545000"/>
+          <a:ext cx="169560" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8928,7 +8928,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="166450" y="45720"/>
+                <a:pt x="169560" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -8969,8 +8969,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1831671" y="3368111"/>
-          <a:ext cx="166450" cy="178934"/>
+          <a:off x="1865888" y="3590720"/>
+          <a:ext cx="169560" cy="182277"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8981,16 +8981,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="178934"/>
+                <a:pt x="0" y="182277"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="83225" y="178934"/>
+                <a:pt x="84780" y="182277"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="83225" y="0"/>
+                <a:pt x="84780" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="166450" y="0"/>
+                <a:pt x="169560" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9031,8 +9031,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="832965" y="2741839"/>
-          <a:ext cx="166450" cy="805206"/>
+          <a:off x="848526" y="2952750"/>
+          <a:ext cx="169560" cy="820248"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9046,13 +9046,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="83225" y="0"/>
+                <a:pt x="84780" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="83225" y="805206"/>
+                <a:pt x="84780" y="820248"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="166450" y="805206"/>
+                <a:pt x="169560" y="820248"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9093,8 +9093,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1831671" y="2652372"/>
-          <a:ext cx="166450" cy="357869"/>
+          <a:off x="1865888" y="2861611"/>
+          <a:ext cx="169560" cy="364554"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9108,13 +9108,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="83225" y="0"/>
+                <a:pt x="84780" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="83225" y="357869"/>
+                <a:pt x="84780" y="364554"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="166450" y="357869"/>
+                <a:pt x="169560" y="364554"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9155,8 +9155,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1831671" y="2606652"/>
-          <a:ext cx="166450" cy="91440"/>
+          <a:off x="1865888" y="2815891"/>
+          <a:ext cx="169560" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9170,7 +9170,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="166450" y="45720"/>
+                <a:pt x="169560" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9211,8 +9211,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1831671" y="2294502"/>
-          <a:ext cx="166450" cy="357869"/>
+          <a:off x="1865888" y="2497056"/>
+          <a:ext cx="169560" cy="364554"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9223,16 +9223,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="357869"/>
+                <a:pt x="0" y="364554"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="83225" y="357869"/>
+                <a:pt x="84780" y="364554"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="83225" y="0"/>
+                <a:pt x="84780" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="166450" y="0"/>
+                <a:pt x="169560" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9273,8 +9273,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="832965" y="2606652"/>
-          <a:ext cx="166450" cy="91440"/>
+          <a:off x="848526" y="2815891"/>
+          <a:ext cx="169560" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9285,16 +9285,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="135187"/>
+                <a:pt x="0" y="136858"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="83225" y="135187"/>
+                <a:pt x="84780" y="136858"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="83225" y="45720"/>
+                <a:pt x="84780" y="45720"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="166450" y="45720"/>
+                <a:pt x="169560" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9335,8 +9335,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4827788" y="2069847"/>
-          <a:ext cx="166450" cy="91440"/>
+          <a:off x="4917975" y="2269059"/>
+          <a:ext cx="169560" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9350,7 +9350,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="166450" y="45720"/>
+                <a:pt x="169560" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9391,8 +9391,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3829082" y="2069847"/>
-          <a:ext cx="166450" cy="91440"/>
+          <a:off x="3900613" y="2269059"/>
+          <a:ext cx="169560" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9406,7 +9406,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="166450" y="45720"/>
+                <a:pt x="169560" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9447,8 +9447,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2830377" y="1936633"/>
-          <a:ext cx="166450" cy="178934"/>
+          <a:off x="2883250" y="2132501"/>
+          <a:ext cx="169560" cy="182277"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9462,13 +9462,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="83225" y="0"/>
+                <a:pt x="84780" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="83225" y="178934"/>
+                <a:pt x="84780" y="182277"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="166450" y="178934"/>
+                <a:pt x="169560" y="182277"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9509,8 +9509,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4827788" y="1711978"/>
-          <a:ext cx="166450" cy="91440"/>
+          <a:off x="4917975" y="1904504"/>
+          <a:ext cx="169560" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9524,7 +9524,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="166450" y="45720"/>
+                <a:pt x="169560" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9565,8 +9565,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3829082" y="1711978"/>
-          <a:ext cx="166450" cy="91440"/>
+          <a:off x="3900613" y="1904504"/>
+          <a:ext cx="169560" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9580,7 +9580,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="166450" y="45720"/>
+                <a:pt x="169560" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9621,8 +9621,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2830377" y="1757698"/>
-          <a:ext cx="166450" cy="178934"/>
+          <a:off x="2883250" y="1950224"/>
+          <a:ext cx="169560" cy="182277"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9633,16 +9633,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="178934"/>
+                <a:pt x="0" y="182277"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="83225" y="178934"/>
+                <a:pt x="84780" y="182277"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="83225" y="0"/>
+                <a:pt x="84780" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="166450" y="0"/>
+                <a:pt x="169560" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9683,8 +9683,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1831671" y="1890913"/>
-          <a:ext cx="166450" cy="91440"/>
+          <a:off x="1865888" y="2086781"/>
+          <a:ext cx="169560" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9698,7 +9698,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="166450" y="45720"/>
+                <a:pt x="169560" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9739,8 +9739,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="832965" y="1936633"/>
-          <a:ext cx="166450" cy="805206"/>
+          <a:off x="848526" y="2132501"/>
+          <a:ext cx="169560" cy="820248"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9751,16 +9751,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="805206"/>
+                <a:pt x="0" y="820248"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="83225" y="805206"/>
+                <a:pt x="84780" y="820248"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="83225" y="0"/>
+                <a:pt x="84780" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="166450" y="0"/>
+                <a:pt x="169560" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -9801,8 +9801,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="711" y="2614920"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="724" y="2823460"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9948,8 +9948,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="711" y="2614920"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="724" y="2823460"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C761AFE1-23FA-4ED4-B755-F211DEC35560}">
@@ -9959,8 +9959,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="999416" y="1809714"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="1018086" y="2003211"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10060,8 +10060,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="999416" y="1809714"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="1018086" y="2003211"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B0A63CB8-EFB4-48AD-A07B-8ECD5D81E20E}">
@@ -10071,8 +10071,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1998122" y="1809714"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="2035448" y="2003211"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10169,8 +10169,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1998122" y="1809714"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="2035448" y="2003211"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{515D5E1F-33CE-4C39-ACA5-DC2E43E68577}">
@@ -10180,8 +10180,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2996827" y="1630779"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="3052811" y="1820934"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10278,8 +10278,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2996827" y="1630779"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="3052811" y="1820934"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{6E733613-3605-4E2D-BC55-623A7C86E222}">
@@ -10289,8 +10289,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3995533" y="1630779"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="4070173" y="1820934"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10387,8 +10387,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3995533" y="1630779"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="4070173" y="1820934"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{043A9824-5113-4919-8600-2DA5529D277C}">
@@ -10398,8 +10398,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4994239" y="1630779"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="5087535" y="1820934"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10496,8 +10496,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4994239" y="1630779"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="5087535" y="1820934"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8922ED77-EBB6-4312-95BF-26E15B0D6022}">
@@ -10507,8 +10507,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2996827" y="1988649"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="3052811" y="2185489"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10605,8 +10605,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2996827" y="1988649"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="3052811" y="2185489"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{CE7A820B-7330-42BA-B4B1-9F5C468A8182}">
@@ -10616,8 +10616,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3995533" y="1988649"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="4070173" y="2185489"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10714,8 +10714,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3995533" y="1988649"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="4070173" y="2185489"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{EACD64C9-36A0-4989-8D19-4D5DA20F07B7}">
@@ -10725,8 +10725,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4994239" y="1988649"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="5087535" y="2185489"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10823,8 +10823,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4994239" y="1988649"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="5087535" y="2185489"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{018F2AAA-1279-487B-BD04-BDF13083DA44}">
@@ -10834,8 +10834,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="999416" y="2525453"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="1018086" y="2732321"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10935,8 +10935,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="999416" y="2525453"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="1018086" y="2732321"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{76DDE225-FC92-4423-A794-254BC00DAA92}">
@@ -10946,8 +10946,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1998122" y="2167583"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="2035448" y="2367766"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11044,8 +11044,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1998122" y="2167583"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="2035448" y="2367766"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8381AAF2-A953-41BD-A42D-CD62E7D23FA5}">
@@ -11055,8 +11055,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1998122" y="2525453"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="2035448" y="2732321"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11153,8 +11153,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1998122" y="2525453"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="2035448" y="2732321"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C44FBF2F-02F4-49EE-9CD3-7D1DD0C90AFA}">
@@ -11164,8 +11164,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1998122" y="2883322"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="2035448" y="3096876"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11262,8 +11262,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1998122" y="2883322"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="2035448" y="3096876"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B11AF780-A2EE-4B9E-B2DF-6499D657D73A}">
@@ -11273,8 +11273,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="999416" y="3420127"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="1018086" y="3643708"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11371,8 +11371,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="999416" y="3420127"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="1018086" y="3643708"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{31C72BBF-7886-427F-8CEB-BC4A97B6E3BA}">
@@ -11382,8 +11382,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1998122" y="3241192"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="2035448" y="3461431"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11480,8 +11480,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1998122" y="3241192"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="2035448" y="3461431"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{283C6606-3838-45BF-8F5D-B8D86B190BEB}">
@@ -11491,8 +11491,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2996827" y="3241192"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="3052811" y="3461431"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11589,8 +11589,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2996827" y="3241192"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="3052811" y="3461431"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{6B224435-D11C-4858-B411-4744171E4F77}">
@@ -11600,8 +11600,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3995533" y="3241192"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="4070173" y="3461431"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11698,8 +11698,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3995533" y="3241192"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="4070173" y="3461431"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{AE2F6C31-C6CC-4B4A-B0FC-FA3C4D53877A}">
@@ -11709,8 +11709,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1998122" y="3599061"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="2035448" y="3825985"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11807,8 +11807,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1998122" y="3599061"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="2035448" y="3825985"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{9BD66DB3-3838-4A96-85D9-EADE83E7D265}">
@@ -11818,8 +11818,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2996827" y="3599061"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="3052811" y="3825985"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11916,8 +11916,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2996827" y="3599061"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="3052811" y="3825985"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{CE72A2D6-5BE1-48C7-BA85-0D3C52B01C89}">
@@ -11927,8 +11927,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3995533" y="3599061"/>
-          <a:ext cx="832254" cy="253837"/>
+          <a:off x="4070173" y="3825985"/>
+          <a:ext cx="847801" cy="258579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12025,8 +12025,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3995533" y="3599061"/>
-        <a:ext cx="832254" cy="253837"/>
+        <a:off x="4070173" y="3825985"/>
+        <a:ext cx="847801" cy="258579"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -12048,8 +12048,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2475596" y="2763"/>
-          <a:ext cx="1580235" cy="1053490"/>
+          <a:off x="2482406" y="1425"/>
+          <a:ext cx="1702686" cy="1135124"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -12124,8 +12124,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2506452" y="33619"/>
-        <a:ext cx="1518523" cy="991778"/>
+        <a:off x="2515653" y="34672"/>
+        <a:ext cx="1636192" cy="1068630"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E30BD6D4-F793-47AE-B571-513DF71DB394}">
@@ -12135,8 +12135,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2238560" y="1056254"/>
-          <a:ext cx="1027153" cy="421396"/>
+          <a:off x="2227003" y="1136550"/>
+          <a:ext cx="1106746" cy="454049"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -12147,16 +12147,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="1027153" y="0"/>
+                <a:pt x="1106746" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1027153" y="210698"/>
+                <a:pt x="1106746" y="227024"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="210698"/>
+                <a:pt x="0" y="227024"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="421396"/>
+                <a:pt x="0" y="454049"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -12197,8 +12197,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1448443" y="1477650"/>
-          <a:ext cx="1580235" cy="1053490"/>
+          <a:off x="1375660" y="1590600"/>
+          <a:ext cx="1702686" cy="1135124"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -12273,8 +12273,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1479299" y="1508506"/>
-        <a:ext cx="1518523" cy="991778"/>
+        <a:off x="1408907" y="1623847"/>
+        <a:ext cx="1636192" cy="1068630"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{2290DF2D-1E9F-404E-968B-B296B2B0A3D0}">
@@ -12284,8 +12284,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2192840" y="2531140"/>
-          <a:ext cx="91440" cy="421396"/>
+          <a:off x="2181283" y="2725724"/>
+          <a:ext cx="91440" cy="454049"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -12299,7 +12299,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="421396"/>
+                <a:pt x="45720" y="454049"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -12340,8 +12340,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1448443" y="2952537"/>
-          <a:ext cx="1580235" cy="1053490"/>
+          <a:off x="1375660" y="3179774"/>
+          <a:ext cx="1702686" cy="1135124"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -12416,8 +12416,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1479299" y="2983393"/>
-        <a:ext cx="1518523" cy="991778"/>
+        <a:off x="1408907" y="3213021"/>
+        <a:ext cx="1636192" cy="1068630"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{CA8135AA-F264-40C6-BEE7-C7492803687B}">
@@ -12427,8 +12427,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2192840" y="4006027"/>
-          <a:ext cx="91440" cy="421396"/>
+          <a:off x="2181283" y="4314898"/>
+          <a:ext cx="91440" cy="454049"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -12442,7 +12442,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="421396"/>
+                <a:pt x="45720" y="454049"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -12483,8 +12483,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1448443" y="4427423"/>
-          <a:ext cx="1580235" cy="1053490"/>
+          <a:off x="1375660" y="4768948"/>
+          <a:ext cx="1702686" cy="1135124"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -12559,8 +12559,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1479299" y="4458279"/>
-        <a:ext cx="1518523" cy="991778"/>
+        <a:off x="1408907" y="4802195"/>
+        <a:ext cx="1636192" cy="1068630"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{1AD8AC4B-6905-4352-B445-5FCDB981CB0D}">
@@ -12570,8 +12570,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3265714" y="1056254"/>
-          <a:ext cx="1027153" cy="421396"/>
+          <a:off x="3333750" y="1136550"/>
+          <a:ext cx="1106746" cy="454049"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -12585,13 +12585,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="210698"/>
+                <a:pt x="0" y="227024"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1027153" y="210698"/>
+                <a:pt x="1106746" y="227024"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1027153" y="421396"/>
+                <a:pt x="1106746" y="454049"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -12632,8 +12632,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3502749" y="1477650"/>
-          <a:ext cx="1580235" cy="1053490"/>
+          <a:off x="3589153" y="1590600"/>
+          <a:ext cx="1702686" cy="1135124"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -12708,8 +12708,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3533605" y="1508506"/>
-        <a:ext cx="1518523" cy="991778"/>
+        <a:off x="3622400" y="1623847"/>
+        <a:ext cx="1636192" cy="1068630"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E580B2E0-3A49-4879-90BE-E84362729CEF}">
@@ -12719,8 +12719,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4247147" y="2531140"/>
-          <a:ext cx="91440" cy="421396"/>
+          <a:off x="4394776" y="2725724"/>
+          <a:ext cx="91440" cy="454049"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -12734,7 +12734,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="421396"/>
+                <a:pt x="45720" y="454049"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -12775,8 +12775,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3502749" y="2952537"/>
-          <a:ext cx="1580235" cy="1053490"/>
+          <a:off x="3589153" y="3179774"/>
+          <a:ext cx="1702686" cy="1135124"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -12851,8 +12851,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3533605" y="2983393"/>
-        <a:ext cx="1518523" cy="991778"/>
+        <a:off x="3622400" y="3213021"/>
+        <a:ext cx="1636192" cy="1068630"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C179BC42-6F1D-4149-AC79-F63EA23BE62D}">
@@ -12862,8 +12862,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4247147" y="4006027"/>
-          <a:ext cx="91440" cy="421396"/>
+          <a:off x="4394776" y="4314898"/>
+          <a:ext cx="91440" cy="454049"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -12877,7 +12877,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="421396"/>
+                <a:pt x="45720" y="454049"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -12918,8 +12918,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3502749" y="4427423"/>
-          <a:ext cx="1580235" cy="1053490"/>
+          <a:off x="3589153" y="4768948"/>
+          <a:ext cx="1702686" cy="1135124"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -12994,8 +12994,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3533605" y="4458279"/>
-        <a:ext cx="1518523" cy="991778"/>
+        <a:off x="3622400" y="4802195"/>
+        <a:ext cx="1636192" cy="1068630"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -13017,8 +13017,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4406198" y="161298"/>
-          <a:ext cx="1129529" cy="753019"/>
+          <a:off x="4491106" y="256192"/>
+          <a:ext cx="1151295" cy="767530"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -13093,8 +13093,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4428253" y="183353"/>
-        <a:ext cx="1085419" cy="708909"/>
+        <a:off x="4513586" y="278672"/>
+        <a:ext cx="1106335" cy="722570"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E30BD6D4-F793-47AE-B571-513DF71DB394}">
@@ -13104,8 +13104,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2034187" y="914317"/>
-          <a:ext cx="2936776" cy="301207"/>
+          <a:off x="2073386" y="1023722"/>
+          <a:ext cx="2993368" cy="307012"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -13116,16 +13116,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="2936776" y="0"/>
+                <a:pt x="2993368" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="2936776" y="150603"/>
+                <a:pt x="2993368" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="150603"/>
+                <a:pt x="0" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="301207"/>
+                <a:pt x="0" y="307012"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -13166,8 +13166,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1469422" y="1215525"/>
-          <a:ext cx="1129529" cy="753019"/>
+          <a:off x="1497738" y="1330734"/>
+          <a:ext cx="1151295" cy="767530"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -13242,8 +13242,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1491477" y="1237580"/>
-        <a:ext cx="1085419" cy="708909"/>
+        <a:off x="1520218" y="1353214"/>
+        <a:ext cx="1106335" cy="722570"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{2290DF2D-1E9F-404E-968B-B296B2B0A3D0}">
@@ -13253,8 +13253,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="565799" y="1968545"/>
-          <a:ext cx="1468388" cy="301207"/>
+          <a:off x="576702" y="2098265"/>
+          <a:ext cx="1496684" cy="307012"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -13265,16 +13265,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="1468388" y="0"/>
+                <a:pt x="1496684" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1468388" y="150603"/>
+                <a:pt x="1496684" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="150603"/>
+                <a:pt x="0" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="301207"/>
+                <a:pt x="0" y="307012"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -13315,8 +13315,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1034" y="2269753"/>
-          <a:ext cx="1129529" cy="753019"/>
+          <a:off x="1054" y="2405277"/>
+          <a:ext cx="1151295" cy="767530"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -13391,8 +13391,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="23089" y="2291808"/>
-        <a:ext cx="1085419" cy="708909"/>
+        <a:off x="23534" y="2427757"/>
+        <a:ext cx="1106335" cy="722570"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{CA8135AA-F264-40C6-BEE7-C7492803687B}">
@@ -13402,8 +13402,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1988467" y="1968545"/>
-          <a:ext cx="91440" cy="301207"/>
+          <a:off x="2027666" y="2098265"/>
+          <a:ext cx="91440" cy="307012"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -13417,7 +13417,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="301207"/>
+                <a:pt x="45720" y="307012"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -13458,8 +13458,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1469422" y="2269753"/>
-          <a:ext cx="1129529" cy="753019"/>
+          <a:off x="1497738" y="2405277"/>
+          <a:ext cx="1151295" cy="767530"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -13534,8 +13534,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1491477" y="2291808"/>
-        <a:ext cx="1085419" cy="708909"/>
+        <a:off x="1520218" y="2427757"/>
+        <a:ext cx="1106335" cy="722570"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{322E84A8-832A-4D06-AAAF-94930DDFC14E}">
@@ -13545,8 +13545,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2034187" y="1968545"/>
-          <a:ext cx="1468388" cy="301207"/>
+          <a:off x="2073386" y="2098265"/>
+          <a:ext cx="1496684" cy="307012"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -13560,13 +13560,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="150603"/>
+                <a:pt x="0" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1468388" y="150603"/>
+                <a:pt x="1496684" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1468388" y="301207"/>
+                <a:pt x="1496684" y="307012"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -13607,8 +13607,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2937810" y="2269753"/>
-          <a:ext cx="1129529" cy="753019"/>
+          <a:off x="2994422" y="2405277"/>
+          <a:ext cx="1151295" cy="767530"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -13683,8 +13683,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2959865" y="2291808"/>
-        <a:ext cx="1085419" cy="708909"/>
+        <a:off x="3016902" y="2427757"/>
+        <a:ext cx="1106335" cy="722570"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{1AD8AC4B-6905-4352-B445-5FCDB981CB0D}">
@@ -13694,8 +13694,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4970963" y="914317"/>
-          <a:ext cx="734194" cy="301207"/>
+          <a:off x="5066754" y="1023722"/>
+          <a:ext cx="748342" cy="307012"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -13709,13 +13709,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="150603"/>
+                <a:pt x="0" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="734194" y="150603"/>
+                <a:pt x="748342" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="734194" y="301207"/>
+                <a:pt x="748342" y="307012"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -13756,8 +13756,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5140392" y="1215525"/>
-          <a:ext cx="1129529" cy="753019"/>
+          <a:off x="5239448" y="1330734"/>
+          <a:ext cx="1151295" cy="767530"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -13832,8 +13832,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5162447" y="1237580"/>
-        <a:ext cx="1085419" cy="708909"/>
+        <a:off x="5261928" y="1353214"/>
+        <a:ext cx="1106335" cy="722570"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E580B2E0-3A49-4879-90BE-E84362729CEF}">
@@ -13843,8 +13843,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4970963" y="1968545"/>
-          <a:ext cx="734194" cy="301207"/>
+          <a:off x="5066754" y="2098265"/>
+          <a:ext cx="748342" cy="307012"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -13855,16 +13855,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="734194" y="0"/>
+                <a:pt x="748342" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="734194" y="150603"/>
+                <a:pt x="748342" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="150603"/>
+                <a:pt x="0" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="301207"/>
+                <a:pt x="0" y="307012"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -13905,8 +13905,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4406198" y="2269753"/>
-          <a:ext cx="1129529" cy="753019"/>
+          <a:off x="4491106" y="2405277"/>
+          <a:ext cx="1151295" cy="767530"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -13981,8 +13981,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4428253" y="2291808"/>
-        <a:ext cx="1085419" cy="708909"/>
+        <a:off x="4513586" y="2427757"/>
+        <a:ext cx="1106335" cy="722570"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C179BC42-6F1D-4149-AC79-F63EA23BE62D}">
@@ -13992,8 +13992,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5705157" y="1968545"/>
-          <a:ext cx="734194" cy="301207"/>
+          <a:off x="5815096" y="2098265"/>
+          <a:ext cx="748342" cy="307012"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -14007,13 +14007,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="150603"/>
+                <a:pt x="0" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="734194" y="150603"/>
+                <a:pt x="748342" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="734194" y="301207"/>
+                <a:pt x="748342" y="307012"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -14054,8 +14054,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5874587" y="2269753"/>
-          <a:ext cx="1129529" cy="753019"/>
+          <a:off x="5987791" y="2405277"/>
+          <a:ext cx="1151295" cy="767530"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -14130,8 +14130,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5896642" y="2291808"/>
-        <a:ext cx="1085419" cy="708909"/>
+        <a:off x="6010271" y="2427757"/>
+        <a:ext cx="1106335" cy="722570"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{4E3B7974-9961-477F-A8AF-7D24D2E5BEF8}">
@@ -14141,8 +14141,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4970963" y="914317"/>
-          <a:ext cx="2936776" cy="301207"/>
+          <a:off x="5066754" y="1023722"/>
+          <a:ext cx="2993368" cy="307012"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -14156,13 +14156,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="150603"/>
+                <a:pt x="0" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="2936776" y="150603"/>
+                <a:pt x="2993368" y="153506"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="2936776" y="301207"/>
+                <a:pt x="2993368" y="307012"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -14203,8 +14203,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7342975" y="1215525"/>
-          <a:ext cx="1129529" cy="753019"/>
+          <a:off x="7484475" y="1330734"/>
+          <a:ext cx="1151295" cy="767530"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -14279,8 +14279,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7365030" y="1237580"/>
-        <a:ext cx="1085419" cy="708909"/>
+        <a:off x="7506955" y="1353214"/>
+        <a:ext cx="1106335" cy="722570"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F97457DE-F1C8-4B53-85C6-549C462B1761}">
@@ -14290,8 +14290,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7862019" y="1968545"/>
-          <a:ext cx="91440" cy="301207"/>
+          <a:off x="8014402" y="2098265"/>
+          <a:ext cx="91440" cy="307012"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -14305,7 +14305,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="301207"/>
+                <a:pt x="45720" y="307012"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -14346,8 +14346,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7342975" y="2269753"/>
-          <a:ext cx="1129529" cy="753019"/>
+          <a:off x="7484475" y="2405277"/>
+          <a:ext cx="1151295" cy="767530"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -14422,8 +14422,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7365030" y="2291808"/>
-        <a:ext cx="1085419" cy="708909"/>
+        <a:off x="7506955" y="2427757"/>
+        <a:ext cx="1106335" cy="722570"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -14445,8 +14445,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2576852" y="0"/>
-          <a:ext cx="1377723" cy="918482"/>
+          <a:off x="2592283" y="1333"/>
+          <a:ext cx="1482932" cy="988621"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -14521,8 +14521,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2603753" y="26901"/>
-        <a:ext cx="1323921" cy="864680"/>
+        <a:off x="2621239" y="30289"/>
+        <a:ext cx="1425020" cy="930709"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E30BD6D4-F793-47AE-B571-513DF71DB394}">
@@ -14532,8 +14532,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2370193" y="918482"/>
-          <a:ext cx="895520" cy="367392"/>
+          <a:off x="2369843" y="989955"/>
+          <a:ext cx="963906" cy="395448"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -14544,16 +14544,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="895520" y="0"/>
+                <a:pt x="963906" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="895520" y="183696"/>
+                <a:pt x="963906" y="197724"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="183696"/>
+                <a:pt x="0" y="197724"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="367392"/>
+                <a:pt x="0" y="395448"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -14594,8 +14594,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1681332" y="1285875"/>
-          <a:ext cx="1377723" cy="918482"/>
+          <a:off x="1628377" y="1385403"/>
+          <a:ext cx="1482932" cy="988621"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -14670,8 +14670,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1708233" y="1312776"/>
-        <a:ext cx="1323921" cy="864680"/>
+        <a:off x="1657333" y="1414359"/>
+        <a:ext cx="1425020" cy="930709"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{2290DF2D-1E9F-404E-968B-B296B2B0A3D0}">
@@ -14681,8 +14681,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2324473" y="2204357"/>
-          <a:ext cx="91440" cy="367392"/>
+          <a:off x="2324123" y="2374025"/>
+          <a:ext cx="91440" cy="395448"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -14696,7 +14696,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="367392"/>
+                <a:pt x="45720" y="395448"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -14737,8 +14737,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1681332" y="2571749"/>
-          <a:ext cx="1377723" cy="918482"/>
+          <a:off x="1628377" y="2769474"/>
+          <a:ext cx="1482932" cy="988621"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -14813,8 +14813,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1708233" y="2598650"/>
-        <a:ext cx="1323921" cy="864680"/>
+        <a:off x="1657333" y="2798430"/>
+        <a:ext cx="1425020" cy="930709"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{CA8135AA-F264-40C6-BEE7-C7492803687B}">
@@ -14824,8 +14824,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2324473" y="3490231"/>
-          <a:ext cx="91440" cy="367392"/>
+          <a:off x="2324123" y="3758096"/>
+          <a:ext cx="91440" cy="395448"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -14839,7 +14839,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="367392"/>
+                <a:pt x="45720" y="395448"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -14880,8 +14880,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1681332" y="3857624"/>
-          <a:ext cx="1377723" cy="918482"/>
+          <a:off x="1628377" y="4153544"/>
+          <a:ext cx="1482932" cy="988621"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -14956,8 +14956,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1708233" y="3884525"/>
-        <a:ext cx="1323921" cy="864680"/>
+        <a:off x="1657333" y="4182500"/>
+        <a:ext cx="1425020" cy="930709"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{1AD8AC4B-6905-4352-B445-5FCDB981CB0D}">
@@ -14967,8 +14967,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3265714" y="918482"/>
-          <a:ext cx="895520" cy="367392"/>
+          <a:off x="3333750" y="989955"/>
+          <a:ext cx="963906" cy="395448"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -14982,13 +14982,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="183696"/>
+                <a:pt x="0" y="197724"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="895520" y="183696"/>
+                <a:pt x="963906" y="197724"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="895520" y="367392"/>
+                <a:pt x="963906" y="395448"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -15029,8 +15029,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3472372" y="1285875"/>
-          <a:ext cx="1377723" cy="918482"/>
+          <a:off x="3556189" y="1385403"/>
+          <a:ext cx="1482932" cy="988621"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -15105,8 +15105,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3499273" y="1312776"/>
-        <a:ext cx="1323921" cy="864680"/>
+        <a:off x="3585145" y="1414359"/>
+        <a:ext cx="1425020" cy="930709"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E580B2E0-3A49-4879-90BE-E84362729CEF}">
@@ -15116,8 +15116,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4115514" y="2204357"/>
-          <a:ext cx="91440" cy="367392"/>
+          <a:off x="4251936" y="2374025"/>
+          <a:ext cx="91440" cy="395448"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -15131,7 +15131,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="367392"/>
+                <a:pt x="45720" y="395448"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -15172,8 +15172,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3472372" y="2571749"/>
-          <a:ext cx="1377723" cy="918482"/>
+          <a:off x="3556189" y="2769474"/>
+          <a:ext cx="1482932" cy="988621"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -15248,8 +15248,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3499273" y="2598650"/>
-        <a:ext cx="1323921" cy="864680"/>
+        <a:off x="3585145" y="2798430"/>
+        <a:ext cx="1425020" cy="930709"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C179BC42-6F1D-4149-AC79-F63EA23BE62D}">
@@ -15259,8 +15259,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4115514" y="3490231"/>
-          <a:ext cx="91440" cy="367392"/>
+          <a:off x="4251936" y="3758096"/>
+          <a:ext cx="91440" cy="395448"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -15274,7 +15274,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="367392"/>
+                <a:pt x="45720" y="395448"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -15315,8 +15315,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3472372" y="3857624"/>
-          <a:ext cx="1377723" cy="918482"/>
+          <a:off x="3556189" y="4153544"/>
+          <a:ext cx="1482932" cy="988621"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -15391,8 +15391,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3499273" y="3884525"/>
-        <a:ext cx="1323921" cy="864680"/>
+        <a:off x="3585145" y="4182500"/>
+        <a:ext cx="1425020" cy="930709"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -15414,8 +15414,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1850186" y="1371929"/>
-          <a:ext cx="2831055" cy="1141591"/>
+          <a:off x="1805135" y="1466594"/>
+          <a:ext cx="3057227" cy="1232792"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -15511,8 +15511,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1883622" y="1405365"/>
-        <a:ext cx="2764183" cy="1074719"/>
+        <a:off x="1841242" y="1502701"/>
+        <a:ext cx="2985013" cy="1160578"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E30BD6D4-F793-47AE-B571-513DF71DB394}">
@@ -15522,8 +15522,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1039610" y="2513520"/>
-          <a:ext cx="2226103" cy="456636"/>
+          <a:off x="929803" y="2699387"/>
+          <a:ext cx="2403945" cy="493117"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -15534,16 +15534,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="2226103" y="0"/>
+                <a:pt x="2403945" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="2226103" y="228318"/>
+                <a:pt x="2403945" y="246558"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="228318"/>
+                <a:pt x="0" y="246558"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="456636"/>
+                <a:pt x="0" y="493117"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -15584,8 +15584,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="183417" y="2970157"/>
-          <a:ext cx="1712387" cy="1141591"/>
+          <a:off x="5208" y="3192504"/>
+          <a:ext cx="1849189" cy="1232792"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -15660,8 +15660,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="216853" y="3003593"/>
-        <a:ext cx="1645515" cy="1074719"/>
+        <a:off x="41315" y="3228611"/>
+        <a:ext cx="1776975" cy="1160578"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{1AD8AC4B-6905-4352-B445-5FCDB981CB0D}">
@@ -15671,8 +15671,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3219994" y="2513520"/>
-          <a:ext cx="91440" cy="456636"/>
+          <a:off x="3288029" y="2699387"/>
+          <a:ext cx="91440" cy="493117"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -15686,7 +15686,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="456636"/>
+                <a:pt x="45720" y="493117"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -15727,8 +15727,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2409520" y="2970157"/>
-          <a:ext cx="1712387" cy="1141591"/>
+          <a:off x="2409154" y="3192504"/>
+          <a:ext cx="1849189" cy="1232792"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -15803,8 +15803,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2442956" y="3003593"/>
-        <a:ext cx="1645515" cy="1074719"/>
+        <a:off x="2445261" y="3228611"/>
+        <a:ext cx="1776975" cy="1160578"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C63F273E-BB71-449A-955A-4AEBC9451165}">
@@ -15814,8 +15814,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3265714" y="2513520"/>
-          <a:ext cx="2226103" cy="456636"/>
+          <a:off x="3333749" y="2699387"/>
+          <a:ext cx="2403945" cy="493117"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -15829,13 +15829,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="228318"/>
+                <a:pt x="0" y="246558"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="2226103" y="228318"/>
+                <a:pt x="2403945" y="246558"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="2226103" y="456636"/>
+                <a:pt x="2403945" y="493117"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -15876,8 +15876,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4635623" y="2970157"/>
-          <a:ext cx="1712387" cy="1141591"/>
+          <a:off x="4813100" y="3192504"/>
+          <a:ext cx="1849189" cy="1232792"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -15952,8 +15952,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4669059" y="3003593"/>
-        <a:ext cx="1645515" cy="1074719"/>
+        <a:off x="4849207" y="3228611"/>
+        <a:ext cx="1776975" cy="1160578"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -29123,8 +29123,8 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>235324</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>13606</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>93568</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
@@ -29134,10 +29134,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="99" name="Group 98">
+        <xdr:cNvPr id="2" name="Group 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F4B5282-3D68-43A8-A865-D1BD3E68807C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{881085CB-D226-4C3E-B373-596B9EB5BFD6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29145,142 +29145,18 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="235324" y="4169970"/>
-          <a:ext cx="6113318" cy="3137406"/>
-          <a:chOff x="235324" y="4316665"/>
-          <a:chExt cx="6140824" cy="3247428"/>
+          <a:off x="235324" y="447354"/>
+          <a:ext cx="6068786" cy="7015886"/>
+          <a:chOff x="235324" y="439932"/>
+          <a:chExt cx="6113318" cy="6867444"/>
         </a:xfrm>
       </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="20" name="Rectangle: Rounded Corners 19">
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="99" name="Group 98">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0117B8B6-73A1-40F8-AE6C-AA44A7D8F117}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="16200000">
-            <a:off x="2112710" y="2439279"/>
-            <a:ext cx="2386051" cy="6140824"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst>
-              <a:gd name="adj" fmla="val 8854"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="none" w="med" len="med"/>
-            <a:tailEnd type="none" w="med" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:lnRef>
-          <a:fillRef idx="2">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-PH" sz="1100">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="29" name="Rectangle: Rounded Corners 28">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C9BBFC3-7C03-478F-8270-BFA0826164CE}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1322294" y="6846916"/>
-            <a:ext cx="3966882" cy="717177"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst>
-              <a:gd name="adj" fmla="val 8854"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent3">
-              <a:lumMod val="20000"/>
-              <a:lumOff val="80000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:headEnd type="none" w="med" len="med"/>
-            <a:tailEnd type="none" w="med" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:lnRef>
-          <a:fillRef idx="2">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-PH" sz="1100" b="1">
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Lakbay:</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-PH" sz="1100" b="1" baseline="0">
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t> A Three-Dimensional Game about Driving Fundamentals and Road Courtesy and Safety of Gear-1 Driving School</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-PH" sz="1100" b="1">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="98" name="Group 97">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5286DDDF-A63B-4418-A5CC-B657705300AB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F4B5282-3D68-43A8-A865-D1BD3E68807C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -29288,18 +29164,70 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="449035" y="4502487"/>
-            <a:ext cx="5682981" cy="1985841"/>
-            <a:chOff x="449035" y="4502487"/>
-            <a:chExt cx="5682981" cy="1985841"/>
+            <a:off x="235324" y="4169970"/>
+            <a:ext cx="6113318" cy="3137406"/>
+            <a:chOff x="235324" y="4316665"/>
+            <a:chExt cx="6140824" cy="3247428"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="28" name="Rectangle: Rounded Corners 27">
+            <xdr:cNvPr id="20" name="Rectangle: Rounded Corners 19">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60215CE7-4E3E-49BB-8250-AF071AE69FB0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0117B8B6-73A1-40F8-AE6C-AA44A7D8F117}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm rot="16200000">
+              <a:off x="2112710" y="2439279"/>
+              <a:ext cx="2386051" cy="6140824"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst>
+                <a:gd name="adj" fmla="val 8854"/>
+              </a:avLst>
+            </a:prstGeom>
+            <a:ln>
+              <a:headEnd type="none" w="med" len="med"/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent6"/>
+            </a:lnRef>
+            <a:fillRef idx="2">
+              <a:schemeClr val="accent6"/>
+            </a:fillRef>
+            <a:effectRef idx="1">
+              <a:schemeClr val="accent6"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-PH" sz="1100">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="29" name="Rectangle: Rounded Corners 28">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C9BBFC3-7C03-478F-8270-BFA0826164CE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -29307,8 +29235,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="449035" y="4502487"/>
-              <a:ext cx="1311087" cy="1972234"/>
+              <a:off x="1322294" y="6846916"/>
+              <a:ext cx="3966882" cy="717177"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
               <a:avLst>
@@ -29346,21 +29274,316 @@
             <a:p>
               <a:pPr algn="ctr"/>
               <a:r>
-                <a:rPr lang="en-PH" sz="1100">
+                <a:rPr lang="en-PH" sz="1100" b="1">
                   <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
-                <a:t>Game Module</a:t>
+                <a:t>Lakbay:</a:t>
               </a:r>
+              <a:r>
+                <a:rPr lang="en-PH" sz="1100" b="1" baseline="0">
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t> A Three-Dimensional Game about Driving Fundamentals and Road Courtesy and Safety of Gear-1 Driving School</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-PH" sz="1100" b="1">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="98" name="Group 97">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5286DDDF-A63B-4418-A5CC-B657705300AB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="449035" y="4502487"/>
+              <a:ext cx="5682981" cy="1985841"/>
+              <a:chOff x="449035" y="4502487"/>
+              <a:chExt cx="5682981" cy="1985841"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="28" name="Rectangle: Rounded Corners 27">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60215CE7-4E3E-49BB-8250-AF071AE69FB0}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="449035" y="4502487"/>
+                <a:ext cx="1311087" cy="1972234"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst>
+                  <a:gd name="adj" fmla="val 8854"/>
+                </a:avLst>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:headEnd type="none" w="med" len="med"/>
+                <a:tailEnd type="none" w="med" len="med"/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="1">
+                <a:schemeClr val="accent6"/>
+              </a:lnRef>
+              <a:fillRef idx="2">
+                <a:schemeClr val="accent6"/>
+              </a:fillRef>
+              <a:effectRef idx="1">
+                <a:schemeClr val="accent6"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="dk1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-PH" sz="1100">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Game Module</a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="30" name="Rectangle: Rounded Corners 29">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F41C33D6-9997-42FA-A124-A75DBE79EAD8}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="1903664" y="4502487"/>
+                <a:ext cx="1311088" cy="1972234"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst>
+                  <a:gd name="adj" fmla="val 8854"/>
+                </a:avLst>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:headEnd type="none" w="med" len="med"/>
+                <a:tailEnd type="none" w="med" len="med"/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="1">
+                <a:schemeClr val="accent6"/>
+              </a:lnRef>
+              <a:fillRef idx="2">
+                <a:schemeClr val="accent6"/>
+              </a:fillRef>
+              <a:effectRef idx="1">
+                <a:schemeClr val="accent6"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="dk1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-PH" sz="1100">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Settings Module</a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="31" name="Rectangle: Rounded Corners 30">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{436E6DE8-CDCD-4AFF-BF11-6980EA5E93FC}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="3366298" y="4516094"/>
+                <a:ext cx="1311087" cy="1972234"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst>
+                  <a:gd name="adj" fmla="val 8854"/>
+                </a:avLst>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:headEnd type="none" w="med" len="med"/>
+                <a:tailEnd type="none" w="med" len="med"/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="1">
+                <a:schemeClr val="accent6"/>
+              </a:lnRef>
+              <a:fillRef idx="2">
+                <a:schemeClr val="accent6"/>
+              </a:fillRef>
+              <a:effectRef idx="1">
+                <a:schemeClr val="accent6"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="dk1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-PH" sz="1100">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Information Module</a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="32" name="Rectangle: Rounded Corners 31">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CAAA30D-1914-4290-8707-F70954C1C73B}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="4820928" y="4502487"/>
+                <a:ext cx="1311088" cy="1972234"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst>
+                  <a:gd name="adj" fmla="val 8854"/>
+                </a:avLst>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:headEnd type="none" w="med" len="med"/>
+                <a:tailEnd type="none" w="med" len="med"/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="1">
+                <a:schemeClr val="accent6"/>
+              </a:lnRef>
+              <a:fillRef idx="2">
+                <a:schemeClr val="accent6"/>
+              </a:fillRef>
+              <a:effectRef idx="1">
+                <a:schemeClr val="accent6"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="dk1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-PH" sz="1100">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Video Module</a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="35" name="Group 34">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{151C888B-01C5-4843-B7EB-38A70401FC76}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="2608203" y="439932"/>
+            <a:ext cx="1340342" cy="1465068"/>
+            <a:chOff x="2617371" y="1419945"/>
+            <a:chExt cx="1349511" cy="1515996"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="30" name="Rectangle: Rounded Corners 29">
+            <xdr:cNvPr id="33" name="Oval 32">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F41C33D6-9997-42FA-A124-A75DBE79EAD8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B85838-F724-4AA7-A29E-2F82B8493299}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -29368,24 +29591,55 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1903664" y="4502487"/>
-              <a:ext cx="1311088" cy="1972234"/>
+              <a:off x="2938341" y="1419945"/>
+              <a:ext cx="715575" cy="717177"/>
             </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst>
-                <a:gd name="adj" fmla="val 8854"/>
-              </a:avLst>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
             </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="20000"/>
-                <a:lumOff val="80000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:headEnd type="none" w="med" len="med"/>
-              <a:tailEnd type="none" w="med" len="med"/>
-            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent6"/>
+            </a:lnRef>
+            <a:fillRef idx="2">
+              <a:schemeClr val="accent6"/>
+            </a:fillRef>
+            <a:effectRef idx="1">
+              <a:schemeClr val="accent6"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-PH" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="34" name="Oval 33">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9B1D400-D52B-4342-869C-6F7AA7A2A5A6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2617371" y="2218765"/>
+              <a:ext cx="1349511" cy="717176"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
           </xdr:spPr>
           <xdr:style>
             <a:lnRef idx="1">
@@ -29411,186 +29665,32 @@
                   <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
-                <a:t>Settings Module</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="31" name="Rectangle: Rounded Corners 30">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{436E6DE8-CDCD-4AFF-BF11-6980EA5E93FC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3366298" y="4516094"/>
-              <a:ext cx="1311087" cy="1972234"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst>
-                <a:gd name="adj" fmla="val 8854"/>
-              </a:avLst>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="20000"/>
-                <a:lumOff val="80000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:headEnd type="none" w="med" len="med"/>
-              <a:tailEnd type="none" w="med" len="med"/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="1">
-              <a:schemeClr val="accent6"/>
-            </a:lnRef>
-            <a:fillRef idx="2">
-              <a:schemeClr val="accent6"/>
-            </a:fillRef>
-            <a:effectRef idx="1">
-              <a:schemeClr val="accent6"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-PH" sz="1100">
-                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                </a:rPr>
-                <a:t>Information Module</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="32" name="Rectangle: Rounded Corners 31">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CAAA30D-1914-4290-8707-F70954C1C73B}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4820928" y="4502487"/>
-              <a:ext cx="1311088" cy="1972234"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst>
-                <a:gd name="adj" fmla="val 8854"/>
-              </a:avLst>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="20000"/>
-                <a:lumOff val="80000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:headEnd type="none" w="med" len="med"/>
-              <a:tailEnd type="none" w="med" len="med"/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="1">
-              <a:schemeClr val="accent6"/>
-            </a:lnRef>
-            <a:fillRef idx="2">
-              <a:schemeClr val="accent6"/>
-            </a:fillRef>
-            <a:effectRef idx="1">
-              <a:schemeClr val="accent6"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-PH" sz="1100">
-                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                </a:rPr>
-                <a:t>Video Module</a:t>
+                <a:t>Player</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
       </xdr:grpSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>633930</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>93568</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="35" name="Group 34">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{151C888B-01C5-4843-B7EB-38A70401FC76}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="2608203" y="439932"/>
-          <a:ext cx="1340342" cy="1465068"/>
-          <a:chOff x="2617371" y="1419945"/>
-          <a:chExt cx="1349511" cy="1515996"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="33" name="Oval 32">
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="72" name="Connector: Elbow 71">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B85838-F724-4AA7-A29E-2F82B8493299}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AC4BDFD-BDCE-4C07-A8B8-6AF83F4032D3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="33" idx="2"/>
+            <a:endCxn id="28" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
         <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2938341" y="1419945"/>
-            <a:ext cx="715575" cy="717177"/>
+          <a:xfrm rot="10800000" flipV="1">
+            <a:off x="1099330" y="786952"/>
+            <a:ext cx="1829081" cy="3562655"/>
           </a:xfrm>
-          <a:prstGeom prst="ellipse">
+          <a:prstGeom prst="bentConnector2">
             <a:avLst/>
           </a:prstGeom>
         </xdr:spPr>
@@ -29598,44 +29698,154 @@
           <a:lnRef idx="1">
             <a:schemeClr val="accent6"/>
           </a:lnRef>
-          <a:fillRef idx="2">
+          <a:fillRef idx="0">
             <a:schemeClr val="accent6"/>
           </a:fillRef>
-          <a:effectRef idx="1">
+          <a:effectRef idx="0">
             <a:schemeClr val="accent6"/>
           </a:effectRef>
           <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
+            <a:schemeClr val="tx1"/>
           </a:fontRef>
         </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-PH" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="75" name="Connector: Elbow 74">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB5E8091-F60E-4472-B039-3A1589678AF5}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="33" idx="6"/>
+            <a:endCxn id="32" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3636201" y="786953"/>
+            <a:ext cx="1818371" cy="3562655"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="78" name="Connector: Elbow 77">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34522874-9326-44E6-9AA0-31BF94A6E501}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="34" idx="2"/>
+            <a:endCxn id="30" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="10800000" flipV="1">
+            <a:off x="2546791" y="1561690"/>
+            <a:ext cx="61412" cy="2787917"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="84" name="Connector: Elbow 83">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2467BB39-DA0B-441B-BEA7-9EE3648FD07A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="34" idx="6"/>
+            <a:endCxn id="31" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3948545" y="1561691"/>
+            <a:ext cx="58566" cy="2801343"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="34" name="Oval 33">
+          <xdr:cNvPr id="89" name="Arrow: Right 88">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9B1D400-D52B-4342-869C-6F7AA7A2A5A6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6846BD65-E693-4E17-A114-16B5C1DF47EA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2617371" y="2218765"/>
-            <a:ext cx="1349511" cy="717176"/>
+          <a:xfrm rot="16200000">
+            <a:off x="614441" y="2983422"/>
+            <a:ext cx="1559857" cy="442103"/>
           </a:xfrm>
-          <a:prstGeom prst="ellipse">
+          <a:prstGeom prst="rightArrow">
             <a:avLst/>
           </a:prstGeom>
+          <a:ln>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
         </xdr:spPr>
         <xdr:style>
           <a:lnRef idx="1">
@@ -29661,801 +29871,416 @@
                 <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:rPr>
-              <a:t>Player</a:t>
+              <a:t>Playability</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>441239</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>94225</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>296047</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>20062</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="72" name="Connector: Elbow 71">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AC4BDFD-BDCE-4C07-A8B8-6AF83F4032D3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="33" idx="2"/>
-          <a:endCxn id="28" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="1094382" y="801796"/>
-          <a:ext cx="1814236" cy="3640587"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>345746</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>94226</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>189845</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>20063</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="75" name="Connector: Elbow 74">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB5E8091-F60E-4472-B039-3A1589678AF5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="33" idx="6"/>
-          <a:endCxn id="32" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3611460" y="801797"/>
-          <a:ext cx="1803528" cy="3640587"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>572518</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>176235</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>633930</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>20062</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="78" name="Connector: Elbow 77">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34522874-9326-44E6-9AA0-31BF94A6E501}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="34" idx="2"/>
-          <a:endCxn id="30" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="2531947" y="1591378"/>
-          <a:ext cx="61412" cy="2851005"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>176236</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>58566</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>33489</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="84" name="Connector: Elbow 83">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2467BB39-DA0B-441B-BEA7-9EE3648FD07A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="34" idx="6"/>
-          <a:endCxn id="31" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3918857" y="1591379"/>
-          <a:ext cx="58566" cy="2864431"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>515227</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>299239</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>174402</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="89" name="Arrow: Right 88">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6846BD65-E693-4E17-A114-16B5C1DF47EA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="581970" y="3124132"/>
-          <a:ext cx="1622202" cy="441237"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100">
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="90" name="Arrow: Left 89">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9D1D8FA-6FF2-4CA7-95B4-89ECC465DC8E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="53463" y="2987317"/>
+            <a:ext cx="1552062" cy="442103"/>
+          </a:xfrm>
+          <a:prstGeom prst="leftArrow">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-PH" sz="1100">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Interact with UI</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="92" name="Arrow: Right 91">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE505628-3742-4187-B2B7-15A8CBBCE5F9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="2052251" y="2987318"/>
+            <a:ext cx="1552065" cy="442103"/>
+          </a:xfrm>
+          <a:prstGeom prst="rightArrow">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-PH" sz="1100">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Apply Changes</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="93" name="Arrow: Left 92">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41947177-0578-4CD9-9AB3-8D51DA549F43}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="1487810" y="2987750"/>
+            <a:ext cx="1552062" cy="441237"/>
+          </a:xfrm>
+          <a:prstGeom prst="leftArrow">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-PH" sz="1100">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Modify Settings</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="94" name="Arrow: Right 93">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C628BC82-B37E-4BD6-AA52-0FE50851D556}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="3514455" y="2989201"/>
+            <a:ext cx="1552064" cy="438338"/>
+          </a:xfrm>
+          <a:prstGeom prst="rightArrow">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-PH" sz="1100">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Read</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-PH" sz="1100" baseline="0">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> Lessons</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-PH" sz="1100">
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Playability</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>608442</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>392454</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>174400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="90" name="Arrow: Left 89">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9D1D8FA-6FF2-4CA7-95B4-89ECC465DC8E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="17960" y="3124131"/>
-          <a:ext cx="1622201" cy="441237"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100">
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="95" name="Arrow: Left 94">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F86B412-8D99-4773-AEE9-E8A92C6F4F94}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="2950013" y="2985868"/>
+            <a:ext cx="1552064" cy="445000"/>
+          </a:xfrm>
+          <a:prstGeom prst="leftArrow">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-PH" sz="1100">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Select</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-PH" sz="1100" baseline="0">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> Lessons</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-PH" sz="1100">
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Interact with UI</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>632959</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180973</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>416971</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>174402</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="92" name="Arrow: Right 91">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE505628-3742-4187-B2B7-15A8CBBCE5F9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="2014151" y="3124131"/>
-          <a:ext cx="1622204" cy="441237"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100">
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="96" name="Arrow: Right 95">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E62B42E-D0D4-43C7-962A-F3F9BF077A29}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="4965742" y="2987318"/>
+            <a:ext cx="1552064" cy="442103"/>
+          </a:xfrm>
+          <a:prstGeom prst="rightArrow">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-PH" sz="1100">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Watch Videos</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="97" name="Arrow: Left 96">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F4B1682-8492-4BFE-81C7-34BD219B34B4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="4399416" y="2985869"/>
+            <a:ext cx="1552064" cy="445002"/>
+          </a:xfrm>
+          <a:prstGeom prst="leftArrow">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-PH" sz="1100">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Select</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-PH" sz="1100" baseline="0">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> Videos</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-PH" sz="1100">
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Apply Changes</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>68949</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>510186</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>174400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="93" name="Arrow: Left 92">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41947177-0578-4CD9-9AB3-8D51DA549F43}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="1450142" y="3124131"/>
-          <a:ext cx="1622201" cy="441237"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Modify Settings</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>122773</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>561111</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>174402</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="94" name="Arrow: Right 93">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C628BC82-B37E-4BD6-AA52-0FE50851D556}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="3474190" y="3125582"/>
-          <a:ext cx="1622203" cy="438338"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Read</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100" baseline="0">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> Lessons</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-PH" sz="1100">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>213090</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180972</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>174400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="95" name="Arrow: Left 94">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F86B412-8D99-4773-AEE9-E8A92C6F4F94}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="2910181" y="3122681"/>
-          <a:ext cx="1622203" cy="444135"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Select</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100" baseline="0">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> Lessons</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-PH" sz="1100">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>255995</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>40007</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>174402</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="96" name="Arrow: Right 95">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E62B42E-D0D4-43C7-962A-F3F9BF077A29}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="4923312" y="3124132"/>
-          <a:ext cx="1622203" cy="441237"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Watch Videos</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>346311</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>133222</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>174402</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="97" name="Arrow: Left 96">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F4B1682-8492-4BFE-81C7-34BD219B34B4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="4357852" y="3122683"/>
-          <a:ext cx="1622203" cy="444136"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Select</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100" baseline="0">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> Videos</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-PH" sz="1100">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -31909,8 +31734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C66C879-C471-4BDA-8A06-3B67B4E2DAFF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="55" zoomScaleNormal="100" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -31947,7 +31772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519B1763-22B4-4AE5-972F-A8B14BEFED7A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="I40" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A9" zoomScale="40" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
       <selection activeCell="U77" sqref="U77"/>
     </sheetView>
   </sheetViews>

</xml_diff>